<commit_message>
update data extraction files and start categorize pressure variables
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Bluemel.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Bluemel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD22788D-A205-41C5-87F5-23EF9132E8B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F521536C-6AB8-47C7-AC2B-709087206181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -4747,7 +4747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4796,12 +4796,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -5379,37 +5373,37 @@
   <dimension ref="A1:AX49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AN3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT49" sqref="AT49"/>
+      <selection pane="bottomRight" activeCell="AX26" sqref="AX26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="120.5546875" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" customWidth="1"/>
-    <col min="19" max="19" width="18.109375" customWidth="1"/>
-    <col min="24" max="25" width="32.6640625" customWidth="1"/>
-    <col min="26" max="26" width="22.5546875" customWidth="1"/>
-    <col min="30" max="30" width="67.6640625" style="11" customWidth="1"/>
-    <col min="34" max="35" width="17.6640625" customWidth="1"/>
-    <col min="36" max="36" width="18.6640625" customWidth="1"/>
-    <col min="37" max="37" width="19.109375" customWidth="1"/>
-    <col min="38" max="38" width="17.6640625" customWidth="1"/>
-    <col min="39" max="39" width="14.33203125" customWidth="1"/>
-    <col min="40" max="40" width="15.88671875" customWidth="1"/>
-    <col min="41" max="41" width="35.33203125" customWidth="1"/>
-    <col min="42" max="42" width="15.44140625" customWidth="1"/>
-    <col min="46" max="46" width="15.109375" customWidth="1"/>
-    <col min="47" max="47" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="120.54296875" customWidth="1"/>
+    <col min="11" max="11" width="26.36328125" customWidth="1"/>
+    <col min="15" max="15" width="17.6328125" customWidth="1"/>
+    <col min="19" max="19" width="18.08984375" customWidth="1"/>
+    <col min="24" max="25" width="32.6328125" customWidth="1"/>
+    <col min="26" max="26" width="22.54296875" customWidth="1"/>
+    <col min="30" max="30" width="67.6328125" style="11" customWidth="1"/>
+    <col min="34" max="35" width="17.6328125" customWidth="1"/>
+    <col min="36" max="36" width="18.6328125" customWidth="1"/>
+    <col min="37" max="37" width="19.08984375" customWidth="1"/>
+    <col min="38" max="38" width="17.6328125" customWidth="1"/>
+    <col min="39" max="39" width="14.36328125" customWidth="1"/>
+    <col min="40" max="40" width="15.90625" customWidth="1"/>
+    <col min="41" max="41" width="35.36328125" customWidth="1"/>
+    <col min="42" max="42" width="15.453125" customWidth="1"/>
+    <col min="46" max="46" width="15.08984375" customWidth="1"/>
+    <col min="47" max="47" width="18.6328125" customWidth="1"/>
     <col min="48" max="48" width="18" customWidth="1"/>
-    <col min="50" max="50" width="87.6640625" style="11" customWidth="1"/>
+    <col min="50" max="50" width="87.6328125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -5475,7 +5469,7 @@
       <c r="AW1" s="15"/>
       <c r="AX1" s="15"/>
     </row>
-    <row r="2" spans="1:50" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -5627,7 +5621,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>241</v>
       </c>
@@ -5685,7 +5679,7 @@
       <c r="AD3"/>
       <c r="AX3"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>256</v>
       </c>
@@ -5822,7 +5816,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>256</v>
       </c>
@@ -5959,7 +5953,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>256</v>
       </c>
@@ -6096,7 +6090,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>256</v>
       </c>
@@ -6233,7 +6227,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>256</v>
       </c>
@@ -6370,7 +6364,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="9" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>264</v>
       </c>
@@ -6498,7 +6492,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="10" spans="1:50" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>272</v>
       </c>
@@ -6629,7 +6623,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>278</v>
       </c>
@@ -6763,7 +6757,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>287</v>
       </c>
@@ -6821,7 +6815,7 @@
       <c r="AD12"/>
       <c r="AX12"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>296</v>
       </c>
@@ -6955,7 +6949,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="14" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>306</v>
       </c>
@@ -7013,7 +7007,7 @@
       <c r="AD14"/>
       <c r="AX14"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>316</v>
       </c>
@@ -7141,7 +7135,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>316</v>
       </c>
@@ -7272,7 +7266,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>316</v>
       </c>
@@ -7403,7 +7397,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>324</v>
       </c>
@@ -7537,7 +7531,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>324</v>
       </c>
@@ -7671,7 +7665,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>324</v>
       </c>
@@ -7805,7 +7799,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>324</v>
       </c>
@@ -7939,7 +7933,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>324</v>
       </c>
@@ -8073,7 +8067,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>335</v>
       </c>
@@ -8192,7 +8186,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>335</v>
       </c>
@@ -8302,7 +8296,7 @@
         <v>520</v>
       </c>
       <c r="AV24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AW24" t="s">
         <v>208</v>
@@ -8311,7 +8305,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>335</v>
       </c>
@@ -8430,7 +8424,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>335</v>
       </c>
@@ -8552,7 +8546,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="27" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>344</v>
       </c>
@@ -8680,7 +8674,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>344</v>
       </c>
@@ -8808,7 +8802,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="29" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>344</v>
       </c>
@@ -8939,7 +8933,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>353</v>
       </c>
@@ -9067,7 +9061,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>353</v>
       </c>
@@ -9195,7 +9189,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="32" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>363</v>
       </c>
@@ -9320,7 +9314,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="33" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>363</v>
       </c>
@@ -9448,7 +9442,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="34" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>372</v>
       </c>
@@ -9576,7 +9570,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="35" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>381</v>
       </c>
@@ -9707,7 +9701,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="36" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>381</v>
       </c>
@@ -9838,7 +9832,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="37" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>391</v>
       </c>
@@ -9963,7 +9957,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="38" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>391</v>
       </c>
@@ -10086,7 +10080,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="39" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>399</v>
       </c>
@@ -10211,7 +10205,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>399</v>
       </c>
@@ -10336,7 +10330,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>406</v>
       </c>
@@ -10394,7 +10388,7 @@
       <c r="AD41"/>
       <c r="AX41"/>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>413</v>
       </c>
@@ -10452,7 +10446,7 @@
       <c r="AD42"/>
       <c r="AX42"/>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>423</v>
       </c>
@@ -10510,7 +10504,7 @@
       <c r="AD43"/>
       <c r="AX43"/>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>432</v>
       </c>
@@ -10571,7 +10565,7 @@
       </c>
       <c r="AX44"/>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>440</v>
       </c>
@@ -10690,7 +10684,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>440</v>
       </c>
@@ -10809,7 +10803,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>440</v>
       </c>
@@ -10928,7 +10922,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>448</v>
       </c>
@@ -11057,7 +11051,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>455</v>
       </c>
@@ -11323,17 +11317,17 @@
       <selection activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="19" max="19" width="32.109375" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.08984375" customWidth="1"/>
+    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" customWidth="1"/>
-    <col min="33" max="33" width="26.33203125" customWidth="1"/>
+    <col min="32" max="32" width="14.6328125" customWidth="1"/>
+    <col min="33" max="33" width="26.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -11398,7 +11392,7 @@
       <c r="AV1" s="9"/>
       <c r="AW1" s="9"/>
     </row>
-    <row r="2" spans="1:49" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -11547,7 +11541,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
       <c r="Q3" t="s">
         <v>21</v>
       </c>
@@ -11604,7 +11598,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
       <c r="Q4" t="s">
         <v>22</v>
       </c>
@@ -11661,7 +11655,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
       <c r="R5" t="s">
         <v>83</v>
       </c>
@@ -11717,7 +11711,7 @@
       </c>
       <c r="AW5" s="8"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.35">
       <c r="R6" t="s">
         <v>84</v>
       </c>
@@ -11762,7 +11756,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="R7" t="s">
         <v>85</v>
       </c>
@@ -11804,7 +11798,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
       <c r="R8" t="s">
         <v>86</v>
       </c>
@@ -11842,7 +11836,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
       <c r="R9" t="s">
         <v>87</v>
       </c>
@@ -11877,7 +11871,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S10" t="s">
         <v>33</v>
       </c>
@@ -11909,7 +11903,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S11" t="s">
         <v>32</v>
       </c>
@@ -11944,7 +11938,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S12" t="s">
         <v>30</v>
       </c>
@@ -11976,7 +11970,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S13" t="s">
         <v>79</v>
       </c>
@@ -12011,7 +12005,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S14" t="s">
         <v>31</v>
       </c>
@@ -12040,7 +12034,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S15" t="s">
         <v>35</v>
       </c>
@@ -12069,7 +12063,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.35">
       <c r="S16" t="s">
         <v>34</v>
       </c>
@@ -12089,7 +12083,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AM17" t="s">
         <v>162</v>
       </c>
@@ -12097,22 +12091,22 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AP18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AP19" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH22" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH23" s="6" t="s">
         <v>115</v>
       </c>
@@ -12147,7 +12141,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH24" t="s">
         <v>129</v>
       </c>
@@ -12173,7 +12167,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH25" t="s">
         <v>137</v>
       </c>
@@ -12196,7 +12190,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AJ26" t="s">
         <v>144</v>
       </c>
@@ -12207,7 +12201,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AJ27" t="s">
         <v>147</v>
       </c>
@@ -12218,7 +12212,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AJ28" t="s">
         <v>149</v>
       </c>
@@ -12226,12 +12220,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AP29" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH30" s="5" t="s">
         <v>151</v>
       </c>
@@ -12254,7 +12248,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH31" s="6" t="s">
         <v>129</v>
       </c>
@@ -12280,7 +12274,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="34:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="34:47" x14ac:dyDescent="0.35">
       <c r="AH32" t="s">
         <v>153</v>
       </c>
@@ -12306,7 +12300,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="33" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AH33" t="s">
         <v>155</v>
       </c>
@@ -12326,7 +12320,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="34" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AI34" t="s">
         <v>157</v>
       </c>
@@ -12341,7 +12335,7 @@
       </c>
       <c r="AX34" s="7"/>
     </row>
-    <row r="35" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="35" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AI35" t="s">
         <v>113</v>
       </c>
@@ -12355,7 +12349,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="36" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AT36" t="s">
         <v>211</v>
       </c>
@@ -12363,10 +12357,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="37" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:50" x14ac:dyDescent="0.3">
+    <row r="38" spans="34:50" x14ac:dyDescent="0.35">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -12394,38 +12388,38 @@
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.36328125" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" customWidth="1"/>
-    <col min="22" max="22" width="18.6640625" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.54296875" customWidth="1"/>
+    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.90625" customWidth="1"/>
+    <col min="19" max="19" width="17.6328125" customWidth="1"/>
+    <col min="20" max="20" width="19.36328125" customWidth="1"/>
+    <col min="21" max="21" width="17.6328125" customWidth="1"/>
+    <col min="22" max="22" width="18.6328125" customWidth="1"/>
+    <col min="25" max="25" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.44140625" customWidth="1"/>
-    <col min="29" max="29" width="15.33203125" customWidth="1"/>
-    <col min="30" max="30" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.6640625" customWidth="1"/>
-    <col min="32" max="32" width="12.5546875" customWidth="1"/>
+    <col min="27" max="27" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.453125" customWidth="1"/>
+    <col min="29" max="29" width="15.36328125" customWidth="1"/>
+    <col min="30" max="30" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.6328125" customWidth="1"/>
+    <col min="32" max="32" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -12471,7 +12465,7 @@
       <c r="AE1" s="15"/>
       <c r="AF1" s="15"/>
     </row>
-    <row r="2" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -12569,7 +12563,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -12635,7 +12629,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -12686,7 +12680,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -12740,7 +12734,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -12782,7 +12776,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -12827,7 +12821,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -12865,7 +12859,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -12903,7 +12897,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -12938,7 +12932,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -12970,7 +12964,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -13002,7 +12996,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -13031,7 +13025,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -13054,7 +13048,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -13080,7 +13074,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -13097,7 +13091,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q17" t="s">
         <v>119</v>
       </c>
@@ -13108,7 +13102,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q18" t="s">
         <v>120</v>
       </c>
@@ -13122,7 +13116,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R19" t="s">
         <v>152</v>
       </c>
@@ -13136,7 +13130,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="17:27" x14ac:dyDescent="0.35">
       <c r="S20" t="s">
         <v>156</v>
       </c>
@@ -13147,7 +13141,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="17:27" x14ac:dyDescent="0.35">
       <c r="S21" t="s">
         <v>228</v>
       </c>
@@ -13161,7 +13155,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="17:27" x14ac:dyDescent="0.35">
       <c r="S22" t="s">
         <v>113</v>
       </c>
@@ -13172,7 +13166,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q23" t="s">
         <v>127</v>
       </c>
@@ -13183,7 +13177,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R24" t="s">
         <v>141</v>
       </c>
@@ -13191,7 +13185,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R25" t="s">
         <v>146</v>
       </c>
@@ -13199,7 +13193,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R26" t="s">
         <v>148</v>
       </c>
@@ -13207,7 +13201,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R27" t="s">
         <v>150</v>
       </c>
@@ -13221,7 +13215,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q28" t="s">
         <v>122</v>
       </c>
@@ -13232,7 +13226,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R29" t="s">
         <v>142</v>
       </c>
@@ -13243,7 +13237,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q30" t="s">
         <v>123</v>
       </c>
@@ -13254,7 +13248,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="17:27" x14ac:dyDescent="0.35">
       <c r="R31" t="s">
         <v>143</v>
       </c>
@@ -13262,7 +13256,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="17:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="17:27" x14ac:dyDescent="0.35">
       <c r="Q32" t="s">
         <v>128</v>
       </c>
@@ -13270,12 +13264,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="25:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y33" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="25:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y34" t="s">
         <v>150</v>
       </c>
@@ -13295,21 +13289,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -13423,30 +13402,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13460,4 +13431,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
T4.1 data cleaning and analysing bycatch case study
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Bluemel.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Bluemel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D0B84-2060-4525-A68A-7640D079484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68565FF0-125F-43BC-95F7-11625C1748C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2870,7 +2870,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="628">
   <si>
     <t>SearchID</t>
   </si>
@@ -4769,6 +4769,9 @@
   </si>
   <si>
     <t xml:space="preserve">Digesta was most prev-elant in the stomachs of dab sampled from the control line, which resulted in a significantly greater SC/FL index for these dab (Fig. 3; K-W, H = 19.9, p &lt; 0.001). A larger number of the stomachs of dab collected on the control lines contained Amphiura spp. arms compared with those of fish collected on the treatment line (Fig. 2; Fisher's exact test, p &lt; 0.001). In contrast, the stom- achs of dab collected from the treatment line con- tained much larger numbers of oral discs of Amphiura spp. than those collected on the control line on 3 con- secutive days after the initial disturbance (Fig. 2; x2 = 228.3, p &lt; 0.001). Immedately after fishing distur-bance, the SC/FL index of dab collected on the treat- ment line had increased significantly since the previ- ous day and was significantly higher than for dab col- lected on the control line (Fig. 3; K-W, H = 7.29, p &lt; 0.008). Thereafter, the SC/FL index did not vary sig- nificantly for dab collected from either treatment or control lines (Fig. 3). </t>
+  </si>
+  <si>
+    <t>fishing effort</t>
   </si>
 </sst>
 </file>
@@ -5416,10 +5419,10 @@
   <dimension ref="A1:AX52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AI42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AO57" sqref="AO57"/>
+      <selection pane="bottomRight" activeCell="AX57" sqref="AX57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5833,7 +5836,7 @@
         <v>162</v>
       </c>
       <c r="AO4" t="s">
-        <v>486</v>
+        <v>627</v>
       </c>
       <c r="AQ4" t="s">
         <v>164</v>
@@ -5848,7 +5851,7 @@
         <v>468</v>
       </c>
       <c r="AV4" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="AW4" t="s">
         <v>207</v>
@@ -5970,7 +5973,7 @@
         <v>162</v>
       </c>
       <c r="AO5" t="s">
-        <v>486</v>
+        <v>627</v>
       </c>
       <c r="AQ5" t="s">
         <v>164</v>
@@ -5985,7 +5988,7 @@
         <v>468</v>
       </c>
       <c r="AV5" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW5" t="s">
         <v>207</v>
@@ -6107,7 +6110,7 @@
         <v>162</v>
       </c>
       <c r="AO6" t="s">
-        <v>486</v>
+        <v>627</v>
       </c>
       <c r="AQ6" t="s">
         <v>164</v>
@@ -6122,7 +6125,7 @@
         <v>468</v>
       </c>
       <c r="AV6" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW6" t="s">
         <v>210</v>
@@ -6244,7 +6247,7 @@
         <v>162</v>
       </c>
       <c r="AO7" t="s">
-        <v>486</v>
+        <v>627</v>
       </c>
       <c r="AQ7" t="s">
         <v>164</v>
@@ -6259,7 +6262,7 @@
         <v>468</v>
       </c>
       <c r="AV7" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW7" t="s">
         <v>210</v>
@@ -6381,7 +6384,7 @@
         <v>162</v>
       </c>
       <c r="AO8" t="s">
-        <v>486</v>
+        <v>627</v>
       </c>
       <c r="AQ8" t="s">
         <v>164</v>
@@ -6396,7 +6399,7 @@
         <v>468</v>
       </c>
       <c r="AV8" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW8" t="s">
         <v>209</v>
@@ -13642,12 +13645,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -13761,6 +13758,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13771,21 +13774,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD9F6DFA-3CE5-417E-90E8-A9FD71AA783B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13801,6 +13789,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>

</xml_diff>